<commit_message>
change get date/time/timestamp object way
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/prepareStatement/sql_ps_batch_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/prepareStatement/sql_ps_batch_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="39">
   <si>
     <t>TestID</t>
   </si>
@@ -42,134 +42,126 @@
     <t>Validation_type</t>
   </si>
   <si>
+    <t>prepareStatement</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Value_type</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>使用prepareStatement批量插入数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>ps_batch_001</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Insert_count</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select count(*) from $schema26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_sql1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_sql2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dml_sql1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_sql3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_result1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_result2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dml_result1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_result3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select count(*) from $schema26 where name='BJ'</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dml_sql2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Dml_result2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete from $schema26</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_sql4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Query_result4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>effected_rows_assert</t>
+  </si>
+  <si>
+    <t>Insert_sql</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>insert into $schema26 values(?,?,?,?,?,?,?,?,?,?,?,?)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Integer,Varchar,Integer,Bigint,Double,Double,Varchar,Date,Time,Timestamp,Varchar,Boolean</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select count(*) from $schema26 where id&gt;4000 and id&lt;=20000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>16000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update $schema26 set name='BJ' where id&gt;4000 and id&lt;=20000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>y</t>
-  </si>
-  <si>
-    <t>prepareStatement</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Value_type</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>使用prepareStatement批量插入数据</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>ps_batch_001</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Insert_count</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>200000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select count(*) from $schema26</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>schema26</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>200000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_sql1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_sql2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select count(*) from $schema26 where id&gt;40000 and id&lt;=200000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>160000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dml_sql1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>update $schema26 set name='BJ' where id&gt;40000 and id&lt;=200000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>160000</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_sql3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_result1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_result2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dml_result1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_result3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>select count(*) from $schema26 where name='BJ'</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dml_sql2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Dml_result2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>delete from $schema26</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_sql4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Query_result4</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>effected_rows_assert</t>
-  </si>
-  <si>
-    <t>Insert_sql</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>insert into $schema26 values(?,?,?,?,?,?,?,?,?,?,?,?)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Integer,Varchar,Integer,Bigint,Double,Double,Varchar,Date,Time,Timestamp,Varchar,Boolean</t>
-    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -542,7 +534,7 @@
   <dimension ref="A1:W2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -588,49 +580,49 @@
         <v>6</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>38</v>
+        <v>31</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="K1" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>19</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="L1" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="N1" s="7" t="s">
+      <c r="R1" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="T1" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="U1" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="O1" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="P1" s="7" t="s">
+      <c r="V1" s="7" t="s">
         <v>28</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>25</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="U1" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="V1" s="7" t="s">
-        <v>35</v>
       </c>
       <c r="W1" s="4" t="s">
         <v>7</v>
@@ -638,67 +630,67 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.15">
       <c r="A2" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D2" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" s="6" t="s">
-        <v>9</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="H2" s="6" t="s">
-        <v>39</v>
+        <v>32</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>14</v>
+        <v>34</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="N2" s="2" t="s">
-        <v>21</v>
+        <v>36</v>
       </c>
       <c r="O2" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="P2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="Q2" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="P2" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q2" s="2" t="s">
+      <c r="R2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="T2" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="U2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="V2" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="W2" s="5" t="s">
         <v>30</v>
-      </c>
-      <c r="R2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="S2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="T2" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="V2" s="2" t="s">
-        <v>36</v>
-      </c>
-      <c r="W2" s="5" t="s">
-        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>